<commit_message>
remove bind_merged_cell from read_only mode
</commit_message>
<xml_diff>
--- a/pyxlsx/tests/data/read_only.xlsx
+++ b/pyxlsx/tests/data/read_only.xlsx
@@ -20,7 +20,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t xml:space="preserve">merged cell</t>
+  </si>
   <si>
     <t xml:space="preserve">formula</t>
   </si>
@@ -37,6 +40,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -96,8 +100,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -118,23 +126,29 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="n">
@@ -143,7 +157,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B4" s="0" t="n">
         <f aca="false">SUM(B1:B3)</f>
@@ -151,6 +165,9 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D1:E2"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>